<commit_message>
Picture preview bug fixed!
</commit_message>
<xml_diff>
--- a/AngularJS-AdsProject/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/AngularJS-AdsProject/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Presian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\AngularJS-AdsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="JS-SPA-Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -399,10 +399,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,11 +753,11 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
A very last commit!
</commit_message>
<xml_diff>
--- a/AngularJS-AdsProject/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/AngularJS-AdsProject/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
@@ -776,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>